<commit_message>
Ora prende il nome di azienda corretto, ma si deve modificare il comportamento delle macro
</commit_message>
<xml_diff>
--- a/PagineHtml/prodotti0.0.xlsx
+++ b/PagineHtml/prodotti0.0.xlsx
@@ -478,7 +478,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Compostable Shipping Labels - Zero Waste &amp; Factory Direct</t>
+          <t>Shenzhen Forever Industrial Co., Ltd.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -505,7 +505,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Fabbrica all'ingrosso imballaggio compostabile personalizzato Polymailer spedizione biodegradabile poli</t>
+          <t>BEIJING DAORI PLASTICS CO., LTD.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -532,7 +532,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Fabbrica Design personalizzato compostabile Poly Mailer imballaggio in plastica Polymailer con il tuo Logo</t>
+          <t>Dongguan Taihong Packaging Co., Ltd.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -559,7 +559,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>certificato</t>
+          <t>Dongguan Ruitai Packaging Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Etichette di spedizione termiche con stampa diretta A6 4x6 con stampa compostabile continua personalizzata in cina</t>
+          <t>Xinyu Yushui High-Tech Co., Ltd.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Autoadesiva doppia patinata compostabile etichetta di trasferimento termico adesivi Eco Friendly qualità Premium etichette di spedizione fornitore</t>
+          <t>Paper Sailing Factory Company for Paper Products</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -636,7 +636,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Etichette di spedizione compostabili con nastro adesivo per etichette termiche 100x150 di alta qualità</t>
+          <t>Shenzhen Kingcolor Paper Co., Ltd.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Etichette di spedizione termica diretta 4x6 pollici 100x150 etichetta di spedizione termica compostabile 100x150 adesivi 4x6 etichette termiche</t>
+          <t>Dongguan Kaijing New Material Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Stampa personalizzata imballaggio compostabile etichetta di avvertenza adesivi adesivi trasparenti stampa etichette ecologiche</t>
+          <t>Huizhou Yi To Culture Media Co., Ltd.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PLA 100% Compostable Certified Packing Label Printing Biodegradable Eco-friendly Durable Waterproof Custom Die Cut Logo Stickers</t>
+          <t>Best Zaza (xiamen) Industrial &amp; Trade Co., Ltd.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Etichette adesive personalizzate A4 carta bianca 25 fogli di spedizione compostabili etichette per la stampa di codici a barre carta termica</t>
+          <t>Zhuhai Topa Paper Co., Ltd.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Etichette di spedizione termica diretta 4x6 pollici 100x150 etichetta di spedizione termica compostabile 100x150 adesivi 4x6 etichette termiche</t>
+          <t>Shandong Luxu Supply Chain Management Co., Ltd.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Viet Nam bollettini compostabili stampati su misura con marchio imballaggi sostenibili per etichette Eco-consapevoli e aziende verdi</t>
+          <t>HOANG MINH EXPORT COMPANY LIMITED</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -821,7 +821,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Etichette personalizzate Mailer borsa biodegradabile per maglietta</t>
+          <t>Shenzhen Greentree Co., Ltd.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Waterproof Compostable 40 X 46mm 30x20 47x25 43x25 50x30 60x40 58x60 58x40 Adhesive Shipping Labels for Food Packaging Jewellery</t>
+          <t>Dongguan Sunkey Paper&amp;Printing Co., Ltd.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Biodegradabile Eco Friendly etichetta per l'imballaggio biodegradabile e facile da usare</t>
+          <t>Fy Packing Material (shanghai) Co., Ltd.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -902,7 +902,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>certificato</t>
+          <t>Ningbo Kunpeng printing co.ltd.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Etichette adesive personalizzate ecologiche impermeabili biodegradabili PLA compostabili per imballaggi alimentari adesivi stampati etichette</t>
+          <t>Shenzhen Dayu Environmental Protection Packaging Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Etichette di spedizione Eco-Friendly-sostenibile, in 8.5x11 e 4x6 misure, ideale per le imprese orientate al verde</t>
+          <t>Shenzhen Sailing Paper Co., Ltd.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Imballaggi sostenibili con marchio Poly mailer compostabili stampati su misura per etichette ecocompatibili e aziende verdi</t>
+          <t>Shenzhen Deyun Printing Products Co., Ltd.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0,0087-0,0259 €</t>
+          <t>0,0259 €</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Vendita diretta in fabbrica etichette adesive biodegradabili ecologiche per imballaggi sostenibili</t>
+          <t>Anhui Jimei Digital Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Etichette fragili ecologiche-carta riciclata, biodegradabile, imballaggio dell'esportazione</t>
+          <t>Shenzhen Forever Industrial Co., Ltd.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Etichette di carta compostabili personalizzate etichette adesive Eco stampate adesivi in carta biodegradabile per imballaggi alimentari</t>
+          <t>Shenzhen Kaiyu Electronic Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Etichette autoadesive in carta riciclabile Eco-Friendly per iniziative verdi di spedizione di imballaggi sostenibili</t>
+          <t>Qingdao Zhongcai Packaging Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Compostabili personalizzato PLA materiale di carta eco etichette adesive stampa personalizzata biodegradabile adesivi per imballaggi alimentari</t>
+          <t>Jiangsu OPT Barcode Label Co., Ltd.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>certificato</t>
+          <t>Shenzhen Rongzhen Label Consumabels Corp., Ltd.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Etichetta adesiva con sigillo biodegradabile compostabile in materiale cartaceo PLA personalizzato compostabile per confezione</t>
+          <t>Jiangmen MST Packaging Co., Ltd.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>certificato</t>
+          <t>Shenzhen Dinghao Paper Product Packaging Corp. Ltd.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Compostabili Custom Pla materiale carta Eco etichette adesive personalizzate stampate adesivi biodegradabili per l'imballaggio alimentare</t>
+          <t>Guangdong Juncheng Printing Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Etichetta di avvertenza biodegradabile per la vendita al dettaglio di abbigliamento ecologico compostabile adesivo rinforzato a base vegetale</t>
+          <t>Shenzhen Fulida Printing Co., Ltd.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Compostabili custom PLA materiale carta eco etichette adesive personalizzate stampate adesivi biodegradabili per l'imballaggio alimentare</t>
+          <t>Shanghai Brightpac Printing Co., Ltd.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1307,7 +1307,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Carta personalizzata compostabile etichette adesive Eco etichette personalizzate stampate adesivi biodegradabili per l'imballaggio alimentare</t>
+          <t>Shenzhen Xinxincai Security Label Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Pellicola di carta di cellulosa trasparente biodegradabile biodegradabile compostabile a base vegetale adesivo personalizzato per imballaggio impermeabile biodegradabile</t>
+          <t>Shenzhen Ownlikes Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Adesivi adesivi personalizzati impermeabili ecologici compostabili PLA etichette adesive per imballaggi alimentari sostenibili-certificati biodegradabili</t>
+          <t>HONG KONG RUNYIN TONGDA CO., LIMITED</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Stampa personalizzata etichetta adesiva con sigillo compostabile trasparente impermeabile semitrasparente in vinile biodegradabile ecologico per il pacchetto</t>
+          <t>Shenzhen Shengtianxin Printing Co., Ltd.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>certificato</t>
+          <t>Dongguan Caihe Printing Co., Ltd.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>certificato</t>
+          <t>Guangdong Baobang Environmental Protection High-Tech Co., Ltd.</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Etichetta organica biodegradabile degli autoadesivi organici dell'etichetta di fabbricazione dell'oem</t>
+          <t>Shenzhen Enjoy Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Eco Friendly BPA libero rotolo di etichette termiche 4x6 forte adesivo di spedizione etichette impermeabili a prova di olio basso MOQ FSC etichette certificate</t>
+          <t>Fujian Hongye Technology Co., Ltd.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Spedizione di alta qualità e etichettatrice 8*10 etichette stampate prezzo del supermercato etichetta di spedizione biodegradabile</t>
+          <t>Shenzhen Sailing Paper Company Limited</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Etichette termiche biodegradabili impermeabili impermeabili a prova di calore, iniziativa compostabile durevole a rifiuti Zero etichette di compostaggio in 6 mesi</t>
+          <t>Hubei Bisheng Paper Industry Co., Ltd.</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Stampa personalizzata etichette alimentari eco-friendly compostabile congelato etichetta di carne adesivo per alimenti etichette di imballaggio per i prodotti del supermercato</t>
+          <t>Shenzhen Coolmate Printing Co., Ltd.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>termici resistenti alle intemperie spedizione veloce etichette di imballaggio per e-commerce logistica</t>
+          <t>Shenzhen He Li Packaging And Printing Products Co., Ltd.</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1623,7 +1623,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Etichetta compostabile personalizzata etichetta per stampante termica biodegradabile con adesivo termico da 4*6 pollici</t>
+          <t>Shenzhen Hangte Technology Development Co., Ltd.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Etichetta bianca con codice a barre termico diretto in fibra di bambù solubile in acqua etichette di imballaggio degradabili rispettose dell'ambiente</t>
+          <t>HONGKONG PURE TECHNOLOGY LIMITED</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>0,0864-0,4317 €</t>
+          <t>0,4317 €</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Etichetta biodegradabile etichetta materiale compostabile adesivo biodegradabile</t>
+          <t>Jinya New Materials Co., Ltd.</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Adesivi biodegradabili ecologici etichette di carta sostenibili per prodotti biologici etichetta adesivo</t>
+          <t>Dongguan Fenglin Printing Co., Ltd.</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Eco Friendly rapida dissoluzione idrosolubile etichetta adesiva Eco-Friendly biodegradabile per la stampa personalizzata di imballaggio del contenitore di alimenti</t>
+          <t>Zhejiang Jingran Trading Co., Limited</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>

</xml_diff>